<commit_message>
fix get only workdays in /availableMR
</commit_message>
<xml_diff>
--- a/TESTt.xlsx
+++ b/TESTt.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\งาน\ฝึกงาน BOTNOI\calendarAPI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49532ACC-E124-4C3E-A02D-ABD9757372E7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7EF84A1-D03F-4FC5-9340-2F3A01E0F5A7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="M" sheetId="1" r:id="rId1"/>
@@ -88,9 +88,6 @@
     <t>AsokeC</t>
   </si>
   <si>
-    <t>AsokeE</t>
-  </si>
-  <si>
     <t>AsokeF</t>
   </si>
   <si>
@@ -164,9 +161,6 @@
   </si>
   <si>
     <t>RecruiterAsokeA</t>
-  </si>
-  <si>
-    <t>RecruiterAsokeB</t>
   </si>
   <si>
     <t>RecruiterAsokeC</t>
@@ -260,6 +254,12 @@
   </si>
   <si>
     <t>panupong</t>
+  </si>
+  <si>
+    <t>Pemadee</t>
+  </si>
+  <si>
+    <t>Khunnapat</t>
   </si>
 </sst>
 </file>
@@ -668,8 +668,8 @@
   </sheetPr>
   <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -702,7 +702,7 @@
         <v>16</v>
       </c>
       <c r="B2" s="24" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C2" s="5">
         <v>5</v>
@@ -719,7 +719,7 @@
         <v>17</v>
       </c>
       <c r="B3" s="24" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C3" s="5">
         <v>4</v>
@@ -744,7 +744,7 @@
         <v>18</v>
       </c>
       <c r="B5" s="24" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C5" s="5">
         <v>4</v>
@@ -758,10 +758,10 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B6" s="24" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C6" s="5">
         <v>4</v>
@@ -775,7 +775,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>19</v>
+        <v>75</v>
       </c>
       <c r="B7" s="24" t="s">
         <v>69</v>
@@ -792,10 +792,10 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B8" s="24" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C8" s="5">
         <v>4</v>
@@ -817,10 +817,10 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B10" s="24" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C10" s="5">
         <v>4</v>
@@ -834,10 +834,10 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B11" s="24" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C11" s="5">
         <v>4</v>
@@ -851,10 +851,10 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B12" s="24" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C12" s="5">
         <v>4</v>
@@ -868,10 +868,10 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B13" s="24" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C13" s="5">
         <v>5</v>
@@ -893,10 +893,10 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B15" s="24" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C15" s="5">
         <v>4</v>
@@ -918,10 +918,10 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B17" s="24" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C17" s="5">
         <v>4</v>
@@ -943,10 +943,10 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B19" s="24" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C19" s="5">
         <v>4</v>
@@ -960,10 +960,10 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B20" s="24" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C20" s="5">
         <v>5</v>
@@ -985,10 +985,10 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B22" s="24" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C22" s="5">
         <v>4</v>
@@ -1002,10 +1002,10 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B23" s="24" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C23" s="5">
         <v>4</v>
@@ -1048,8 +1048,8 @@
   </sheetPr>
   <dimension ref="A1:Z995"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1125,13 +1125,13 @@
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B3" s="24" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C3" s="18" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D3" s="17"/>
       <c r="E3" s="17"/>
@@ -1159,13 +1159,13 @@
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
-        <v>45</v>
+        <v>76</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C4" s="18" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D4" s="17"/>
       <c r="E4" s="17"/>
@@ -1193,13 +1193,13 @@
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A5" s="18" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B5" s="24" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C5" s="18" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D5" s="17"/>
       <c r="E5" s="17"/>
@@ -1227,13 +1227,13 @@
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6" s="18" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B6" s="24" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C6" s="18" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D6" s="17"/>
       <c r="E6" s="17"/>
@@ -1261,13 +1261,13 @@
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A7" s="18" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B7" s="24" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D7" s="17"/>
       <c r="E7" s="17"/>
@@ -1325,14 +1325,14 @@
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A9" s="18" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B9" s="18" t="str">
         <f t="shared" ref="B9:B21" si="0">A9 &amp; "@mockup.com"</f>
         <v>RecruiterPhuketE@mockup.com</v>
       </c>
       <c r="C9" s="18" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D9" s="17"/>
       <c r="E9" s="17"/>
@@ -1390,14 +1390,14 @@
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A11" s="18" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B11" s="18" t="str">
         <f t="shared" si="0"/>
         <v>RecruiterPattayaF@mockup.com</v>
       </c>
       <c r="C11" s="18" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D11" s="17"/>
       <c r="E11" s="17"/>
@@ -1455,14 +1455,14 @@
     </row>
     <row r="13" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A13" s="18" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B13" s="18" t="str">
         <f t="shared" si="0"/>
         <v>RecruiterSamuiG@mockup.com</v>
       </c>
       <c r="C13" s="18" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D13" s="17"/>
       <c r="E13" s="17"/>
@@ -1520,14 +1520,14 @@
     </row>
     <row r="15" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A15" s="18" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B15" s="18" t="str">
         <f t="shared" si="0"/>
         <v>RecruiterHuahinH@mockup.com</v>
       </c>
       <c r="C15" s="18" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D15" s="17"/>
       <c r="E15" s="17"/>
@@ -1585,14 +1585,14 @@
     </row>
     <row r="17" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A17" s="18" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B17" s="18" t="str">
         <f t="shared" si="0"/>
         <v>RecruiterChiangmaiI@mockup.com</v>
       </c>
       <c r="C17" s="18" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D17" s="17"/>
       <c r="E17" s="17"/>
@@ -1620,14 +1620,14 @@
     </row>
     <row r="18" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A18" s="18" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B18" s="18" t="str">
         <f t="shared" si="0"/>
         <v>RecruiterChiangmaiJ@mockup.com</v>
       </c>
       <c r="C18" s="18" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D18" s="17"/>
       <c r="E18" s="17"/>
@@ -1655,14 +1655,14 @@
     </row>
     <row r="19" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A19" s="18" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B19" s="18" t="str">
         <f t="shared" si="0"/>
         <v>RecruiterChiangmaiK@mockup.com</v>
       </c>
       <c r="C19" s="18" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D19" s="17"/>
       <c r="E19" s="17"/>
@@ -1690,14 +1690,14 @@
     </row>
     <row r="20" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A20" s="18" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B20" s="18" t="str">
         <f t="shared" si="0"/>
         <v>RecruiterChiangmaiL@mockup.com</v>
       </c>
       <c r="C20" s="18" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D20" s="17"/>
       <c r="E20" s="17"/>
@@ -1725,14 +1725,14 @@
     </row>
     <row r="21" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A21" s="18" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B21" s="18" t="str">
         <f t="shared" si="0"/>
         <v>RecruiterChiangmaiM@mockup.com</v>
       </c>
       <c r="C21" s="18" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D21" s="17"/>
       <c r="E21" s="17"/>

</xml_diff>

<commit_message>
change to DB and add auto refresh token func
</commit_message>
<xml_diff>
--- a/TESTt.xlsx
+++ b/TESTt.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\งาน\ฝึกงาน BOTNOI\calendarAPI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7EF84A1-D03F-4FC5-9340-2F3A01E0F5A7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{473E9766-91D8-4F8B-A61E-081D82994C54}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="M" sheetId="1" r:id="rId1"/>
@@ -668,8 +668,8 @@
   </sheetPr>
   <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1048,8 +1048,8 @@
   </sheetPr>
   <dimension ref="A1:Z995"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -29033,9 +29033,9 @@
   </sheetData>
   <phoneticPr fontId="7" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="B6" r:id="rId1" xr:uid="{31A93216-10CA-4192-A918-EB023B2FB873}"/>
-    <hyperlink ref="B5" r:id="rId2" xr:uid="{FC5FD774-7CC6-4EDC-BD22-7522D421BB78}"/>
-    <hyperlink ref="B7" r:id="rId3" xr:uid="{23DAC81B-1342-4CEE-89F1-6BF0B5FB02B0}"/>
+    <hyperlink ref="B5" r:id="rId1" xr:uid="{FC5FD774-7CC6-4EDC-BD22-7522D421BB78}"/>
+    <hyperlink ref="B7" r:id="rId2" xr:uid="{23DAC81B-1342-4CEE-89F1-6BF0B5FB02B0}"/>
+    <hyperlink ref="B6" r:id="rId3" xr:uid="{31A93216-10CA-4192-A918-EB023B2FB873}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Save current changes before rebase
</commit_message>
<xml_diff>
--- a/TESTt.xlsx
+++ b/TESTt.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\งาน\ฝึกงาน BOTNOI\calendarAPI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{473E9766-91D8-4F8B-A61E-081D82994C54}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91A17229-197A-4F99-89B5-F16488842584}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="76">
   <si>
     <t>Silom</t>
   </si>
@@ -143,9 +143,6 @@
   </si>
   <si>
     <t>K@mockup.com</t>
-  </si>
-  <si>
-    <t>L@mockup.com</t>
   </si>
   <si>
     <t>M@mockup.com</t>
@@ -669,7 +666,7 @@
   <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -758,10 +755,10 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B6" s="24" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C6" s="5">
         <v>4</v>
@@ -775,10 +772,10 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B7" s="24" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C7" s="5">
         <v>5</v>
@@ -921,7 +918,7 @@
         <v>25</v>
       </c>
       <c r="B17" s="24" t="s">
-        <v>38</v>
+        <v>68</v>
       </c>
       <c r="C17" s="5">
         <v>4</v>
@@ -946,7 +943,7 @@
         <v>26</v>
       </c>
       <c r="B19" s="24" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C19" s="5">
         <v>4</v>
@@ -963,7 +960,7 @@
         <v>27</v>
       </c>
       <c r="B20" s="24" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C20" s="5">
         <v>5</v>
@@ -988,7 +985,7 @@
         <v>28</v>
       </c>
       <c r="B22" s="24" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C22" s="5">
         <v>4</v>
@@ -1005,7 +1002,7 @@
         <v>29</v>
       </c>
       <c r="B23" s="24" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C23" s="5">
         <v>4</v>
@@ -1027,15 +1024,15 @@
     <hyperlink ref="B8" r:id="rId6" xr:uid="{711506AF-CA03-434A-A11C-B32CA2CA6B56}"/>
     <hyperlink ref="B10:B13" r:id="rId7" display="B@mockup.com" xr:uid="{EE35E3DF-F1B4-4690-85DF-F18056494550}"/>
     <hyperlink ref="B15" r:id="rId8" xr:uid="{3C083FB7-54D4-40C3-BF84-F60507542EA8}"/>
-    <hyperlink ref="B17" r:id="rId9" xr:uid="{8B8C877E-CF3C-4614-876B-BBFE79755B93}"/>
-    <hyperlink ref="B19" r:id="rId10" xr:uid="{B2A1B6D2-94C0-4AF6-A16B-1D714ABE7A08}"/>
-    <hyperlink ref="B20" r:id="rId11" xr:uid="{E0B7EE1F-D684-4766-8BDA-938D747319B0}"/>
-    <hyperlink ref="B22" r:id="rId12" xr:uid="{4217C318-D801-475D-B91E-A20190B03BF8}"/>
-    <hyperlink ref="B23" r:id="rId13" xr:uid="{6D70D49D-C3C2-46F1-B74C-B4CBDD946850}"/>
-    <hyperlink ref="B10" r:id="rId14" xr:uid="{4E5AFCE6-00B1-4840-8D0E-ED422574D417}"/>
-    <hyperlink ref="B11" r:id="rId15" xr:uid="{5E2D272C-62F0-43AC-97B0-F065E64923A0}"/>
-    <hyperlink ref="B12" r:id="rId16" xr:uid="{A289DC81-8133-4E8F-9665-B36F97BF2FFB}"/>
-    <hyperlink ref="B13" r:id="rId17" xr:uid="{F897B959-F075-4A98-A01E-FA47B2C0A36A}"/>
+    <hyperlink ref="B19" r:id="rId9" xr:uid="{B2A1B6D2-94C0-4AF6-A16B-1D714ABE7A08}"/>
+    <hyperlink ref="B20" r:id="rId10" xr:uid="{E0B7EE1F-D684-4766-8BDA-938D747319B0}"/>
+    <hyperlink ref="B22" r:id="rId11" xr:uid="{4217C318-D801-475D-B91E-A20190B03BF8}"/>
+    <hyperlink ref="B23" r:id="rId12" xr:uid="{6D70D49D-C3C2-46F1-B74C-B4CBDD946850}"/>
+    <hyperlink ref="B10" r:id="rId13" xr:uid="{4E5AFCE6-00B1-4840-8D0E-ED422574D417}"/>
+    <hyperlink ref="B11" r:id="rId14" xr:uid="{5E2D272C-62F0-43AC-97B0-F065E64923A0}"/>
+    <hyperlink ref="B12" r:id="rId15" xr:uid="{A289DC81-8133-4E8F-9665-B36F97BF2FFB}"/>
+    <hyperlink ref="B13" r:id="rId16" xr:uid="{F897B959-F075-4A98-A01E-FA47B2C0A36A}"/>
+    <hyperlink ref="B17" r:id="rId17" xr:uid="{576E7977-D703-4604-96C0-A84D565D2AB2}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1049,7 +1046,7 @@
   <dimension ref="A1:Z995"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1125,13 +1122,13 @@
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B3" s="24" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C3" s="18" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D3" s="17"/>
       <c r="E3" s="17"/>
@@ -1159,13 +1156,13 @@
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C4" s="18" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D4" s="17"/>
       <c r="E4" s="17"/>
@@ -1193,13 +1190,13 @@
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A5" s="18" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B5" s="24" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C5" s="18" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D5" s="17"/>
       <c r="E5" s="17"/>
@@ -1227,13 +1224,13 @@
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6" s="18" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B6" s="24" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C6" s="18" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D6" s="17"/>
       <c r="E6" s="17"/>
@@ -1261,13 +1258,13 @@
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A7" s="18" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B7" s="24" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D7" s="17"/>
       <c r="E7" s="17"/>
@@ -1325,14 +1322,14 @@
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A9" s="18" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B9" s="18" t="str">
         <f t="shared" ref="B9:B21" si="0">A9 &amp; "@mockup.com"</f>
         <v>RecruiterPhuketE@mockup.com</v>
       </c>
       <c r="C9" s="18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D9" s="17"/>
       <c r="E9" s="17"/>
@@ -1390,14 +1387,14 @@
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A11" s="18" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B11" s="18" t="str">
         <f t="shared" si="0"/>
         <v>RecruiterPattayaF@mockup.com</v>
       </c>
       <c r="C11" s="18" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D11" s="17"/>
       <c r="E11" s="17"/>
@@ -1455,14 +1452,13 @@
     </row>
     <row r="13" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A13" s="18" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
-      <c r="B13" s="18" t="str">
-        <f t="shared" si="0"/>
-        <v>RecruiterSamuiG@mockup.com</v>
+      <c r="B13" s="24" t="s">
+        <v>69</v>
       </c>
       <c r="C13" s="18" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D13" s="17"/>
       <c r="E13" s="17"/>
@@ -1520,14 +1516,14 @@
     </row>
     <row r="15" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A15" s="18" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B15" s="18" t="str">
         <f t="shared" si="0"/>
         <v>RecruiterHuahinH@mockup.com</v>
       </c>
       <c r="C15" s="18" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D15" s="17"/>
       <c r="E15" s="17"/>
@@ -1585,14 +1581,14 @@
     </row>
     <row r="17" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A17" s="18" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B17" s="18" t="str">
         <f t="shared" si="0"/>
         <v>RecruiterChiangmaiI@mockup.com</v>
       </c>
       <c r="C17" s="18" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D17" s="17"/>
       <c r="E17" s="17"/>
@@ -1620,14 +1616,14 @@
     </row>
     <row r="18" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A18" s="18" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B18" s="18" t="str">
         <f t="shared" si="0"/>
         <v>RecruiterChiangmaiJ@mockup.com</v>
       </c>
       <c r="C18" s="18" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D18" s="17"/>
       <c r="E18" s="17"/>
@@ -1655,14 +1651,14 @@
     </row>
     <row r="19" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A19" s="18" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B19" s="18" t="str">
         <f t="shared" si="0"/>
         <v>RecruiterChiangmaiK@mockup.com</v>
       </c>
       <c r="C19" s="18" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D19" s="17"/>
       <c r="E19" s="17"/>
@@ -1690,14 +1686,14 @@
     </row>
     <row r="20" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A20" s="18" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B20" s="18" t="str">
         <f t="shared" si="0"/>
         <v>RecruiterChiangmaiL@mockup.com</v>
       </c>
       <c r="C20" s="18" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D20" s="17"/>
       <c r="E20" s="17"/>
@@ -1725,14 +1721,14 @@
     </row>
     <row r="21" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A21" s="18" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B21" s="18" t="str">
         <f t="shared" si="0"/>
         <v>RecruiterChiangmaiM@mockup.com</v>
       </c>
       <c r="C21" s="18" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D21" s="17"/>
       <c r="E21" s="17"/>
@@ -29036,6 +29032,7 @@
     <hyperlink ref="B5" r:id="rId1" xr:uid="{FC5FD774-7CC6-4EDC-BD22-7522D421BB78}"/>
     <hyperlink ref="B7" r:id="rId2" xr:uid="{23DAC81B-1342-4CEE-89F1-6BF0B5FB02B0}"/>
     <hyperlink ref="B6" r:id="rId3" xr:uid="{31A93216-10CA-4192-A918-EB023B2FB873}"/>
+    <hyperlink ref="B13" r:id="rId4" xr:uid="{ADD35423-BF17-4B0F-B40C-FA66A014E98F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
add api for viewing and revoking
</commit_message>
<xml_diff>
--- a/TESTt.xlsx
+++ b/TESTt.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\botnoiTN\calendarAPI\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\งาน\ฝึกงาน BOTNOI\calendarAPI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01215FD3-CAC0-4C08-8451-11AADC04DF9A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{340A3613-0412-428A-B750-010BD5F4BC3F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="M" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="76">
   <si>
     <t>Silom</t>
   </si>
@@ -145,9 +145,6 @@
     <t>K@mockup.com</t>
   </si>
   <si>
-    <t>L@mockup.com</t>
-  </si>
-  <si>
     <t>M@mockup.com</t>
   </si>
   <si>
@@ -235,6 +232,9 @@
     <t>0827703801p@gmail.com</t>
   </si>
   <si>
+    <t>khunnapatt65@gmail.com</t>
+  </si>
+  <si>
     <t>pemadee2546@gmail.com</t>
   </si>
   <si>
@@ -256,10 +256,7 @@
     <t>Pemadee</t>
   </si>
   <si>
-    <t>panupongnu4@gmail.com</t>
-  </si>
-  <si>
-    <t>nu4</t>
+    <t>Khunnapat</t>
   </si>
 </sst>
 </file>
@@ -668,8 +665,8 @@
   </sheetPr>
   <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -769,8 +766,8 @@
       <c r="D6" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="6">
-        <v>47</v>
+      <c r="E6" s="6" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -921,7 +918,7 @@
         <v>25</v>
       </c>
       <c r="B17" s="24" t="s">
-        <v>38</v>
+        <v>68</v>
       </c>
       <c r="C17" s="5">
         <v>3</v>
@@ -929,8 +926,8 @@
       <c r="D17" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="E17" s="7" t="s">
-        <v>6</v>
+      <c r="E17" s="7">
+        <v>25</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -946,7 +943,7 @@
         <v>26</v>
       </c>
       <c r="B19" s="24" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C19" s="5">
         <v>3</v>
@@ -963,7 +960,7 @@
         <v>27</v>
       </c>
       <c r="B20" s="24" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C20" s="5">
         <v>4</v>
@@ -988,7 +985,7 @@
         <v>28</v>
       </c>
       <c r="B22" s="24" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C22" s="5">
         <v>3</v>
@@ -1005,7 +1002,7 @@
         <v>29</v>
       </c>
       <c r="B23" s="24" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C23" s="5">
         <v>3</v>
@@ -1027,15 +1024,15 @@
     <hyperlink ref="B8" r:id="rId6" xr:uid="{711506AF-CA03-434A-A11C-B32CA2CA6B56}"/>
     <hyperlink ref="B10:B13" r:id="rId7" display="B@mockup.com" xr:uid="{EE35E3DF-F1B4-4690-85DF-F18056494550}"/>
     <hyperlink ref="B15" r:id="rId8" xr:uid="{3C083FB7-54D4-40C3-BF84-F60507542EA8}"/>
-    <hyperlink ref="B17" r:id="rId9" xr:uid="{8B8C877E-CF3C-4614-876B-BBFE79755B93}"/>
-    <hyperlink ref="B19" r:id="rId10" xr:uid="{B2A1B6D2-94C0-4AF6-A16B-1D714ABE7A08}"/>
-    <hyperlink ref="B20" r:id="rId11" xr:uid="{E0B7EE1F-D684-4766-8BDA-938D747319B0}"/>
-    <hyperlink ref="B22" r:id="rId12" xr:uid="{4217C318-D801-475D-B91E-A20190B03BF8}"/>
-    <hyperlink ref="B23" r:id="rId13" xr:uid="{6D70D49D-C3C2-46F1-B74C-B4CBDD946850}"/>
-    <hyperlink ref="B10" r:id="rId14" xr:uid="{4E5AFCE6-00B1-4840-8D0E-ED422574D417}"/>
-    <hyperlink ref="B11" r:id="rId15" xr:uid="{5E2D272C-62F0-43AC-97B0-F065E64923A0}"/>
-    <hyperlink ref="B12" r:id="rId16" xr:uid="{A289DC81-8133-4E8F-9665-B36F97BF2FFB}"/>
-    <hyperlink ref="B13" r:id="rId17" xr:uid="{F897B959-F075-4A98-A01E-FA47B2C0A36A}"/>
+    <hyperlink ref="B19" r:id="rId9" xr:uid="{B2A1B6D2-94C0-4AF6-A16B-1D714ABE7A08}"/>
+    <hyperlink ref="B20" r:id="rId10" xr:uid="{E0B7EE1F-D684-4766-8BDA-938D747319B0}"/>
+    <hyperlink ref="B22" r:id="rId11" xr:uid="{4217C318-D801-475D-B91E-A20190B03BF8}"/>
+    <hyperlink ref="B23" r:id="rId12" xr:uid="{6D70D49D-C3C2-46F1-B74C-B4CBDD946850}"/>
+    <hyperlink ref="B10" r:id="rId13" xr:uid="{4E5AFCE6-00B1-4840-8D0E-ED422574D417}"/>
+    <hyperlink ref="B11" r:id="rId14" xr:uid="{5E2D272C-62F0-43AC-97B0-F065E64923A0}"/>
+    <hyperlink ref="B12" r:id="rId15" xr:uid="{A289DC81-8133-4E8F-9665-B36F97BF2FFB}"/>
+    <hyperlink ref="B13" r:id="rId16" xr:uid="{F897B959-F075-4A98-A01E-FA47B2C0A36A}"/>
+    <hyperlink ref="B17" r:id="rId17" xr:uid="{576E7977-D703-4604-96C0-A84D565D2AB2}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1048,8 +1045,8 @@
   </sheetPr>
   <dimension ref="A1:Z995"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1125,13 +1122,13 @@
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B3" s="24" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C3" s="18" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D3" s="17"/>
       <c r="E3" s="17"/>
@@ -1159,13 +1156,13 @@
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
-        <v>76</v>
-      </c>
-      <c r="B4" s="24" t="s">
         <v>75</v>
       </c>
+      <c r="B4" s="18" t="s">
+        <v>67</v>
+      </c>
       <c r="C4" s="18" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D4" s="17"/>
       <c r="E4" s="17"/>
@@ -1193,13 +1190,13 @@
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A5" s="18" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B5" s="24" t="s">
         <v>68</v>
       </c>
       <c r="C5" s="18" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D5" s="17"/>
       <c r="E5" s="17"/>
@@ -1233,7 +1230,7 @@
         <v>72</v>
       </c>
       <c r="C6" s="18" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D6" s="17"/>
       <c r="E6" s="17"/>
@@ -1267,7 +1264,7 @@
         <v>68</v>
       </c>
       <c r="C7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D7" s="17"/>
       <c r="E7" s="17"/>
@@ -1325,14 +1322,14 @@
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A9" s="18" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B9" s="18" t="str">
         <f t="shared" ref="B9:B21" si="0">A9 &amp; "@mockup.com"</f>
         <v>RecruiterPhuketE@mockup.com</v>
       </c>
       <c r="C9" s="18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D9" s="17"/>
       <c r="E9" s="17"/>
@@ -1390,14 +1387,14 @@
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A11" s="18" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B11" s="18" t="str">
         <f t="shared" si="0"/>
         <v>RecruiterPattayaF@mockup.com</v>
       </c>
       <c r="C11" s="18" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D11" s="17"/>
       <c r="E11" s="17"/>
@@ -1455,14 +1452,13 @@
     </row>
     <row r="13" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A13" s="18" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
-      <c r="B13" s="18" t="str">
-        <f t="shared" si="0"/>
-        <v>RecruiterSamuiG@mockup.com</v>
+      <c r="B13" s="24" t="s">
+        <v>66</v>
       </c>
       <c r="C13" s="18" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D13" s="17"/>
       <c r="E13" s="17"/>
@@ -1520,14 +1516,14 @@
     </row>
     <row r="15" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A15" s="18" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B15" s="18" t="str">
         <f t="shared" si="0"/>
         <v>RecruiterHuahinH@mockup.com</v>
       </c>
       <c r="C15" s="18" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D15" s="17"/>
       <c r="E15" s="17"/>
@@ -1585,14 +1581,14 @@
     </row>
     <row r="17" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A17" s="18" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B17" s="18" t="str">
         <f t="shared" si="0"/>
         <v>RecruiterChiangmaiI@mockup.com</v>
       </c>
       <c r="C17" s="18" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D17" s="17"/>
       <c r="E17" s="17"/>
@@ -1620,14 +1616,14 @@
     </row>
     <row r="18" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A18" s="18" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B18" s="18" t="str">
         <f t="shared" si="0"/>
         <v>RecruiterChiangmaiJ@mockup.com</v>
       </c>
       <c r="C18" s="18" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D18" s="17"/>
       <c r="E18" s="17"/>
@@ -1655,14 +1651,14 @@
     </row>
     <row r="19" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A19" s="18" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B19" s="18" t="str">
         <f t="shared" si="0"/>
         <v>RecruiterChiangmaiK@mockup.com</v>
       </c>
       <c r="C19" s="18" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D19" s="17"/>
       <c r="E19" s="17"/>
@@ -1690,14 +1686,14 @@
     </row>
     <row r="20" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A20" s="18" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B20" s="18" t="str">
         <f t="shared" si="0"/>
         <v>RecruiterChiangmaiL@mockup.com</v>
       </c>
       <c r="C20" s="18" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D20" s="17"/>
       <c r="E20" s="17"/>
@@ -1725,14 +1721,14 @@
     </row>
     <row r="21" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A21" s="18" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B21" s="18" t="str">
         <f t="shared" si="0"/>
         <v>RecruiterChiangmaiM@mockup.com</v>
       </c>
       <c r="C21" s="18" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D21" s="17"/>
       <c r="E21" s="17"/>
@@ -29033,10 +29029,9 @@
   </sheetData>
   <phoneticPr fontId="7" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="B6" r:id="rId1" xr:uid="{31A93216-10CA-4192-A918-EB023B2FB873}"/>
-    <hyperlink ref="B5" r:id="rId2" xr:uid="{FC5FD774-7CC6-4EDC-BD22-7522D421BB78}"/>
-    <hyperlink ref="B7" r:id="rId3" xr:uid="{23DAC81B-1342-4CEE-89F1-6BF0B5FB02B0}"/>
-    <hyperlink ref="B4" r:id="rId4" xr:uid="{A780D158-8CEE-41AC-B973-02E0835D50CC}"/>
+    <hyperlink ref="B5" r:id="rId1" xr:uid="{FC5FD774-7CC6-4EDC-BD22-7522D421BB78}"/>
+    <hyperlink ref="B7" r:id="rId2" xr:uid="{23DAC81B-1342-4CEE-89F1-6BF0B5FB02B0}"/>
+    <hyperlink ref="B6" r:id="rId3" xr:uid="{31A93216-10CA-4192-A918-EB023B2FB873}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>